<commit_message>
2022-12-06 Resource, World juniours
</commit_message>
<xml_diff>
--- a/Python/World Juniors 2023/price per seat.xlsx
+++ b/Python/World Juniors 2023/price per seat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Important documents\World Juniors 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE436B21-97D9-4E92-A930-4776809FD622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EACEFF6-2966-42C6-A8A8-DA11A5B0A06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{477D85CC-6EC8-47F4-93E0-B8BDEC267BF1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{477D85CC-6EC8-47F4-93E0-B8BDEC267BF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -745,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A116F226-56BF-4CC3-B0E7-9B595D53655A}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2880,7 +3000,7 @@
         <v>64.102564102564102</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" ref="D41:N47" si="38">D$2/$B$41</f>
+        <f t="shared" ref="D41:N42" si="38">D$2/$B$41</f>
         <v>61.53846153846154</v>
       </c>
       <c r="E41" s="2">
@@ -2929,31 +3049,31 @@
         <v>40</v>
       </c>
       <c r="C42" s="2">
-        <f>C$2/$B$42</f>
+        <f t="shared" ref="C42:I42" si="39">C$2/$B$42</f>
         <v>62.5</v>
       </c>
       <c r="D42" s="2">
-        <f>D$2/$B$42</f>
+        <f t="shared" si="39"/>
         <v>60</v>
       </c>
       <c r="E42" s="2">
-        <f>E$2/$B$42</f>
+        <f t="shared" si="39"/>
         <v>57.5</v>
       </c>
       <c r="F42" s="2">
-        <f>F$2/$B$42</f>
+        <f t="shared" si="39"/>
         <v>55</v>
       </c>
       <c r="G42" s="4">
-        <f>G$2/$B$42</f>
+        <f t="shared" si="39"/>
         <v>52.5</v>
       </c>
       <c r="H42" s="2">
-        <f>H$2/$B$42</f>
+        <f t="shared" si="39"/>
         <v>50</v>
       </c>
       <c r="I42" s="2">
-        <f>I$2/$B$42</f>
+        <f t="shared" si="39"/>
         <v>47.5</v>
       </c>
       <c r="J42" s="2">
@@ -2982,51 +3102,51 @@
         <v>41</v>
       </c>
       <c r="C43" s="2">
-        <f>C$2/$B$43</f>
+        <f t="shared" ref="C43:N43" si="40">C$2/$B$43</f>
         <v>60.975609756097562</v>
       </c>
       <c r="D43" s="2">
-        <f>D$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>58.536585365853661</v>
       </c>
       <c r="E43" s="2">
-        <f>E$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>56.097560975609753</v>
       </c>
       <c r="F43" s="2">
-        <f>F$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>53.658536585365852</v>
       </c>
       <c r="G43" s="4">
-        <f>G$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>51.219512195121951</v>
       </c>
       <c r="H43" s="2">
-        <f>H$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>48.780487804878049</v>
       </c>
       <c r="I43" s="2">
-        <f>I$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>46.341463414634148</v>
       </c>
       <c r="J43" s="2">
-        <f>J$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>43.902439024390247</v>
       </c>
       <c r="K43" s="2">
-        <f>K$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>41.463414634146339</v>
       </c>
       <c r="L43" s="2">
-        <f>L$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>39.024390243902438</v>
       </c>
       <c r="M43" s="2">
-        <f>M$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>36.585365853658537</v>
       </c>
       <c r="N43" s="2">
-        <f>N$2/$B$43</f>
+        <f t="shared" si="40"/>
         <v>34.146341463414636</v>
       </c>
     </row>
@@ -3035,51 +3155,51 @@
         <v>42</v>
       </c>
       <c r="C44" s="2">
-        <f>C$2/$B$44</f>
+        <f t="shared" ref="C44:N44" si="41">C$2/$B$44</f>
         <v>59.523809523809526</v>
       </c>
       <c r="D44" s="2">
-        <f>D$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>57.142857142857146</v>
       </c>
       <c r="E44" s="2">
-        <f>E$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>54.761904761904759</v>
       </c>
       <c r="F44" s="2">
-        <f>F$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>52.38095238095238</v>
       </c>
       <c r="G44" s="4">
-        <f>G$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>50</v>
       </c>
       <c r="H44" s="2">
-        <f>H$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>47.61904761904762</v>
       </c>
       <c r="I44" s="2">
-        <f>I$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>45.238095238095241</v>
       </c>
       <c r="J44" s="2">
-        <f>J$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>42.857142857142854</v>
       </c>
       <c r="K44" s="2">
-        <f>K$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>40.476190476190474</v>
       </c>
       <c r="L44" s="2">
-        <f>L$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>38.095238095238095</v>
       </c>
       <c r="M44" s="2">
-        <f>M$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>35.714285714285715</v>
       </c>
       <c r="N44" s="2">
-        <f>N$2/$B$44</f>
+        <f t="shared" si="41"/>
         <v>33.333333333333336</v>
       </c>
     </row>
@@ -3088,47 +3208,47 @@
         <v>43</v>
       </c>
       <c r="C45" s="2">
-        <f>C$2/$B$45</f>
+        <f t="shared" ref="C45:M45" si="42">C$2/$B$45</f>
         <v>58.139534883720927</v>
       </c>
       <c r="D45" s="2">
-        <f>D$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>55.813953488372093</v>
       </c>
       <c r="E45" s="2">
-        <f>E$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>53.488372093023258</v>
       </c>
       <c r="F45" s="2">
-        <f>F$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>51.162790697674417</v>
       </c>
       <c r="G45" s="4">
-        <f>G$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>48.837209302325583</v>
       </c>
       <c r="H45" s="2">
-        <f>H$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>46.511627906976742</v>
       </c>
       <c r="I45" s="2">
-        <f>I$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>44.186046511627907</v>
       </c>
       <c r="J45" s="2">
-        <f>J$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>41.860465116279073</v>
       </c>
       <c r="K45" s="2">
-        <f>K$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>39.534883720930232</v>
       </c>
       <c r="L45" s="2">
-        <f>L$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>37.209302325581397</v>
       </c>
       <c r="M45" s="2">
-        <f>M$2/$B$45</f>
+        <f t="shared" si="42"/>
         <v>34.883720930232556</v>
       </c>
       <c r="N45" s="2">
@@ -3141,47 +3261,47 @@
         <v>44</v>
       </c>
       <c r="C46" s="2">
-        <f>C$2/$B$46</f>
+        <f t="shared" ref="C46:M46" si="43">C$2/$B$46</f>
         <v>56.81818181818182</v>
       </c>
       <c r="D46" s="2">
-        <f>D$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>54.545454545454547</v>
       </c>
       <c r="E46" s="2">
-        <f>E$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>52.272727272727273</v>
       </c>
       <c r="F46" s="2">
-        <f>F$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>50</v>
       </c>
       <c r="G46" s="4">
-        <f>G$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>47.727272727272727</v>
       </c>
       <c r="H46" s="2">
-        <f>H$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>45.454545454545453</v>
       </c>
       <c r="I46" s="2">
-        <f>I$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>43.18181818181818</v>
       </c>
       <c r="J46" s="2">
-        <f>J$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>40.909090909090907</v>
       </c>
       <c r="K46" s="2">
-        <f>K$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>38.636363636363633</v>
       </c>
       <c r="L46" s="2">
-        <f>L$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>36.363636363636367</v>
       </c>
       <c r="M46" s="2">
-        <f>M$2/$B$46</f>
+        <f t="shared" si="43"/>
         <v>34.090909090909093</v>
       </c>
       <c r="N46" s="2">
@@ -3194,88 +3314,406 @@
         <v>45</v>
       </c>
       <c r="C47" s="2">
-        <f>C$2/$B$47</f>
+        <f t="shared" ref="C47:N47" si="44">C$2/$B$47</f>
         <v>55.555555555555557</v>
       </c>
       <c r="D47" s="2">
-        <f>D$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>53.333333333333336</v>
       </c>
       <c r="E47" s="2">
-        <f>E$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>51.111111111111114</v>
       </c>
       <c r="F47" s="2">
-        <f>F$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>48.888888888888886</v>
       </c>
       <c r="G47" s="4">
-        <f>G$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>46.666666666666664</v>
       </c>
       <c r="H47" s="2">
-        <f>H$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>44.444444444444443</v>
       </c>
       <c r="I47" s="2">
-        <f>I$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>42.222222222222221</v>
       </c>
       <c r="J47" s="2">
-        <f>J$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>40</v>
       </c>
       <c r="K47" s="2">
-        <f>K$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>37.777777777777779</v>
       </c>
       <c r="L47" s="2">
-        <f>L$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>35.555555555555557</v>
       </c>
       <c r="M47" s="2">
-        <f>M$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>33.333333333333336</v>
       </c>
       <c r="N47" s="2">
-        <f>N$2/$B$47</f>
+        <f t="shared" si="44"/>
         <v>31.111111111111111</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50">
+    <row r="48" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="1">
+        <v>46</v>
+      </c>
+      <c r="C48" s="2">
+        <f t="shared" ref="C48:N48" si="45">C$2/$B$48</f>
+        <v>54.347826086956523</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="45"/>
+        <v>52.173913043478258</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" si="45"/>
+        <v>47.826086956521742</v>
+      </c>
+      <c r="G48" s="4">
+        <f t="shared" si="45"/>
+        <v>45.652173913043477</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="45"/>
+        <v>43.478260869565219</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="45"/>
+        <v>41.304347826086953</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="45"/>
+        <v>39.130434782608695</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="45"/>
+        <v>36.956521739130437</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" si="45"/>
+        <v>34.782608695652172</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="45"/>
+        <v>32.608695652173914</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="45"/>
+        <v>30.434782608695652</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>47</v>
+      </c>
+      <c r="C49" s="2">
+        <f t="shared" ref="C49:N49" si="46">C$2/$B$49</f>
+        <v>53.191489361702125</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="46"/>
+        <v>51.063829787234042</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="46"/>
+        <v>48.936170212765958</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" si="46"/>
+        <v>46.808510638297875</v>
+      </c>
+      <c r="G49" s="4">
+        <f t="shared" si="46"/>
+        <v>44.680851063829785</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="46"/>
+        <v>42.553191489361701</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="46"/>
+        <v>40.425531914893618</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="46"/>
+        <v>38.297872340425535</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="46"/>
+        <v>36.170212765957444</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="46"/>
+        <v>34.042553191489361</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="46"/>
+        <v>31.914893617021278</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="46"/>
+        <v>29.787234042553191</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <v>48</v>
+      </c>
+      <c r="C50" s="2">
+        <f t="shared" ref="C50:N50" si="47">C$2/$B$50</f>
+        <v>52.083333333333336</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="47"/>
+        <v>50</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="47"/>
+        <v>47.916666666666664</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" si="47"/>
+        <v>45.833333333333336</v>
+      </c>
+      <c r="G50" s="4">
+        <f t="shared" si="47"/>
+        <v>43.75</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="47"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="47"/>
+        <v>39.583333333333336</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="47"/>
+        <v>37.5</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="47"/>
+        <v>35.416666666666664</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="47"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="47"/>
+        <v>31.25</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="47"/>
+        <v>29.166666666666668</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
+        <v>49</v>
+      </c>
+      <c r="C51" s="2">
+        <f t="shared" ref="C51:N51" si="48">C$2/$B$51</f>
+        <v>51.020408163265309</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="48"/>
+        <v>48.979591836734691</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="48"/>
+        <v>46.938775510204081</v>
+      </c>
+      <c r="F51" s="2">
+        <f t="shared" si="48"/>
+        <v>44.897959183673471</v>
+      </c>
+      <c r="G51" s="4">
+        <f t="shared" si="48"/>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="48"/>
+        <v>40.816326530612244</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="48"/>
+        <v>38.775510204081634</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="48"/>
+        <v>36.734693877551024</v>
+      </c>
+      <c r="K51" s="2">
+        <f t="shared" si="48"/>
+        <v>34.693877551020407</v>
+      </c>
+      <c r="L51" s="2">
+        <f t="shared" si="48"/>
+        <v>32.653061224489797</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="48"/>
+        <v>30.612244897959183</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="48"/>
+        <v>28.571428571428573</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
+        <v>50</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" ref="C52:N52" si="49">C$2/$B$52</f>
+        <v>50</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="49"/>
+        <v>48</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="49"/>
+        <v>46</v>
+      </c>
+      <c r="F52" s="2">
+        <f t="shared" si="49"/>
+        <v>44</v>
+      </c>
+      <c r="G52" s="4">
+        <f t="shared" si="49"/>
+        <v>42</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="49"/>
+        <v>40</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="49"/>
+        <v>38</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="49"/>
+        <v>36</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="49"/>
+        <v>34</v>
+      </c>
+      <c r="L52" s="2">
+        <f t="shared" si="49"/>
+        <v>32</v>
+      </c>
+      <c r="M52" s="2">
+        <f t="shared" si="49"/>
+        <v>30</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="49"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="1">
+        <v>51</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" ref="C53:N53" si="50">C$2/$B$53</f>
+        <v>49.019607843137258</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="50"/>
+        <v>47.058823529411768</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="50"/>
+        <v>45.098039215686278</v>
+      </c>
+      <c r="F53" s="2">
+        <f t="shared" si="50"/>
+        <v>43.137254901960787</v>
+      </c>
+      <c r="G53" s="4">
+        <f t="shared" si="50"/>
+        <v>41.176470588235297</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="50"/>
+        <v>39.215686274509807</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="50"/>
+        <v>37.254901960784316</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="50"/>
+        <v>35.294117647058826</v>
+      </c>
+      <c r="K53" s="2">
+        <f t="shared" si="50"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="L53" s="2">
+        <f t="shared" si="50"/>
+        <v>31.372549019607842</v>
+      </c>
+      <c r="M53" s="2">
+        <f t="shared" si="50"/>
+        <v>29.411764705882351</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="50"/>
+        <v>27.450980392156861</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C58">
         <f>(1.15*575*3)</f>
         <v>1983.75</v>
       </c>
-      <c r="E50">
+      <c r="E58">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C59">
         <f>605.48</f>
         <v>605.48</v>
       </c>
-      <c r="D51">
-        <f>C51*1.15</f>
+      <c r="D59">
+        <f>C59*1.15</f>
         <v>696.30200000000002</v>
       </c>
-      <c r="E51" s="3">
-        <f>D51*E50</f>
+      <c r="E59" s="3">
+        <f>D59*E58</f>
         <v>2088.9059999999999</v>
       </c>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C60">
         <v>682.6</v>
       </c>
-      <c r="D52">
-        <f>C52*1.15</f>
+      <c r="D60">
+        <f>C60*1.15</f>
         <v>784.99</v>
       </c>
-      <c r="E52" s="3">
-        <f>D52*E50</f>
+      <c r="E60" s="3">
+        <f>D60*E58</f>
         <v>2354.9700000000003</v>
       </c>
     </row>
@@ -3285,7 +3723,7 @@
     <mergeCell ref="B1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:N41">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="135">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3295,7 +3733,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="136">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3305,7 +3743,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3315,21 +3753,21 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="54" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="139" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="55" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="140" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="56" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="141" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $A$2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:N42">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3339,7 +3777,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3349,7 +3787,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3359,21 +3797,21 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="41" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="126" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="42" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="127" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="128" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $A$2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:N43">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3383,7 +3821,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3393,7 +3831,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3403,21 +3841,21 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="35" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="120" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="121" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="122" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $A$2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:N44">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3427,7 +3865,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3437,7 +3875,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="113">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3447,21 +3885,21 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="114" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="115" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="116" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $A$2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:N45">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3471,7 +3909,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3481,7 +3919,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3491,21 +3929,21 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="108" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="109" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="110" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $A$2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:N46">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3515,7 +3953,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3525,7 +3963,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3535,21 +3973,21 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="102" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="103" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="104" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $A$2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:N47">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3559,7 +3997,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="percentile" val="25"/>
         <cfvo type="percentile" val="50"/>
@@ -3569,7 +4007,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3579,20 +4017,368 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="90" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="91" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $P$3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="92" operator="between">
       <formula>"$P$2 - $P$3"</formula>
       <formula>"$P$2 + $A$2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:N47">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:N48">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="85"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="75"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="76" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="77" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="78" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $A$2"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:N48">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:N49">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="85"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="75"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="69" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="70" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="71" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $A$2"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:N49">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:N50">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="85"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="75"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="62" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="63" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="64" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $A$2"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:N50">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:N51">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="85"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="75"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="27" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="28" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="29" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $A$2"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:N51">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:N52">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="85"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="75"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="20" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="21" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="22" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $A$2"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:N52">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53:N53">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="85"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="75"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $P$3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="between">
+      <formula>"$P$2 - $P$3"</formula>
+      <formula>"$P$2 + $A$2"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53:N53">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:N53">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percentile" val="10"/>

</xml_diff>